<commit_message>
Updated the evaluation script + Finished the Android and Weka sections in Technologies used
</commit_message>
<xml_diff>
--- a/dissertation/Evaluation_Dataset.xlsx
+++ b/dissertation/Evaluation_Dataset.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="345" windowWidth="27555" windowHeight="12555"/>
+    <workbookView xWindow="720" yWindow="345" windowWidth="27555" windowHeight="12555" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="97">
   <si>
     <t>'The Mysterious Affair at Styles'</t>
   </si>
@@ -1139,8 +1140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3073,4 +3074,58 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.5703125" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>